<commit_message>
Updated Recipe Sheets for Hydroxyproline Assay Protocol
Saved old version of recipe sheets and added to "Legacy" folder
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/Stock_Solns/OxidationBuffer_soln_recipe.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/Stock_Solns/OxidationBuffer_soln_recipe.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\Stock_Solns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C144E2-BD49-411D-A367-B4D8749FC0A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20999BF3-0FE5-49AB-9ABD-2DC03E8CC40C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nephorology" sheetId="1" r:id="rId1"/>
-    <sheet name="Brown, et al." sheetId="3" r:id="rId2"/>
+    <sheet name="Brown, et al." sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Brown, et al.'!$A$19:$J$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Nephorology!$A$1:$J$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Brown, et al.'!$A$19:$J$32</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Made by</t>
   </si>
@@ -68,10 +66,6 @@
   </si>
   <si>
     <t>Target pH = 6.00</t>
-  </si>
-  <si>
-    <t>Tri-Sodium Citrate
-Dihydrate</t>
   </si>
   <si>
     <t>Sodium Acetate
@@ -118,9 +112,6 @@
 250mL</t>
   </si>
   <si>
-    <t>38.5mL</t>
-  </si>
-  <si>
     <t>Fill to
 200mL</t>
   </si>
@@ -131,9 +122,6 @@
   <si>
     <t>Fill up to
 250mL</t>
-  </si>
-  <si>
-    <t>Total HCl / NaOH added</t>
   </si>
   <si>
     <t>Sodium Hydroxide</t>
@@ -161,10 +149,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -565,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -649,9 +636,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,6 +655,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,9 +689,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -725,107 +709,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21D443B4-0C35-4853-A46E-DD41FDAF8F8F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2266950" y="66675"/>
-          <a:ext cx="2266950" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Store in 4°C.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Shelf</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> life: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>6 months.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1222,284 +1105,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:J18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="35">
-        <v>136.08000000000001</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="16">
-        <f>I5*2.5</f>
-        <v>14.25</v>
-      </c>
-      <c r="I5" s="16">
-        <v>5.7</v>
-      </c>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="35">
-        <v>294.10000000000002</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0.998</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="16">
-        <f t="shared" ref="H6:H7" si="0">I6*2.5</f>
-        <v>9.375</v>
-      </c>
-      <c r="I6" s="16">
-        <v>3.75</v>
-      </c>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="35">
-        <v>192.124</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0.999</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="16">
-        <f t="shared" si="0"/>
-        <v>1.375</v>
-      </c>
-      <c r="I7" s="16">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="38">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="H8" s="16">
-        <f>38.5*2.5</f>
-        <v>96.25</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="34"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="44"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
-      <c r="B15" s="46"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="48"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:10" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="28"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832A8B93-63E2-4E83-844D-62A66B231B59}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1507,7 +1112,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1527,7 +1132,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="40"/>
     </row>
@@ -1566,10 +1171,10 @@
         <v>7</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="21" t="s">
         <v>10</v>
@@ -1577,11 +1182,11 @@
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>136.08000000000001</v>
       </c>
       <c r="E5" s="9">
@@ -1604,11 +1209,11 @@
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <v>192.124</v>
       </c>
       <c r="E6" s="9">
@@ -1631,11 +1236,11 @@
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>294.10000000000002</v>
       </c>
       <c r="E7" s="9">
@@ -1658,19 +1263,19 @@
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="37"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J8" s="13"/>
     </row>
@@ -1726,7 +1331,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="44"/>
     </row>
@@ -1741,7 +1346,7 @@
     <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -1750,10 +1355,10 @@
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" s="28"/>
     </row>
@@ -1799,10 +1404,10 @@
         <v>7</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>10</v>
@@ -1810,11 +1415,11 @@
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="35"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="9"/>
       <c r="F23" s="17"/>
       <c r="G23" s="9"/>
@@ -1829,42 +1434,42 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="49">
+      <c r="D24" s="35"/>
+      <c r="E24" s="38">
         <v>1</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="38">
+      <c r="F24" s="31"/>
+      <c r="G24" s="37">
         <v>0.38500000000000001</v>
       </c>
       <c r="H24" s="16">
         <v>113.63639999999999</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="32">
         <f>H24/2.5</f>
         <v>45.454560000000001</v>
       </c>
-      <c r="J24" s="34"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="37"/>
+      <c r="D25" s="36"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J25" s="13"/>
     </row>
@@ -1889,7 +1494,7 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="44"/>
     </row>
@@ -1919,6 +1524,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -2141,22 +1761,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A161E6A-5B3F-4912-ADEE-71AD0FF6FC00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2173,29 +1803,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>